<commit_message>
Add more to title column
</commit_message>
<xml_diff>
--- a/edgar/EPV/DOMI.xlsx
+++ b/edgar/EPV/DOMI.xlsx
@@ -34,7 +34,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -43,12 +43,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00dedede"/>
-        <bgColor rgb="00dedede"/>
+        <fgColor rgb="00999997"/>
+        <bgColor rgb="00999997"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ebebeb"/>
+        <bgColor rgb="00ebebeb"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -56,13 +62,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -446,18 +493,157 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:B3"/>
+  <dimension ref="B2:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
+    <row r="2">
+      <c r="B2" s="1" t="inlineStr"/>
+    </row>
     <row r="3">
-      <c r="B3" s="1" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>Operating Income</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Depreciation Adjustment</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Depreciation</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>CAPEX</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Growth CAPEX</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Option Expense</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>Interest Earned on Cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>Interest Rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>Pretax Earnings</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>Tax Rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>Taxes</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Earnings</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>Earnings Power Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>Debt</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>Total EV in Equity</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Shares Outstanding</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>EPV/share</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>Current Share Price</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add formatting for epv data
</commit_message>
<xml_diff>
--- a/edgar/EPV/DOMI.xlsx
+++ b/edgar/EPV/DOMI.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,8 +33,14 @@
       <color rgb="00000000"/>
       <sz val="10"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <strike val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -55,6 +61,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00fef2cc"/>
+        <bgColor rgb="00fef2cc"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="007eab76"/>
         <bgColor rgb="007eab76"/>
       </patternFill>
@@ -65,8 +77,14 @@
         <bgColor rgb="00c6e6c1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00cfe2f3"/>
+        <bgColor rgb="00cfe2f3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -113,7 +131,7 @@
       </bottom>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color rgb="00000000"/>
       </left>
       <right style="thin">
@@ -147,6 +165,40 @@
         <color rgb="00000000"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
       <top/>
       <bottom style="thick">
         <color rgb="00000000"/>
@@ -156,16 +208,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -549,7 +609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C22"/>
+  <dimension ref="B2:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -725,6 +785,114 @@
       </c>
       <c r="C22" s="8" t="inlineStr"/>
     </row>
+    <row r="24">
+      <c r="B24" s="9" t="inlineStr">
+        <is>
+          <t>Premises and Equipment</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="inlineStr">
+        <is>
+          <t>Premises and Equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="11" t="inlineStr">
+        <is>
+          <t>Current Year Revenue</t>
+        </is>
+      </c>
+      <c r="C25" s="12" t="inlineStr">
+        <is>
+          <t>Current Year Revenue</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="11" t="inlineStr">
+        <is>
+          <t>Prior Year Revenue</t>
+        </is>
+      </c>
+      <c r="C26" s="12" t="inlineStr">
+        <is>
+          <t>Prior Year Revenue</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="11" t="inlineStr">
+        <is>
+          <t>Change in Revenue</t>
+        </is>
+      </c>
+      <c r="C27" s="12" t="inlineStr">
+        <is>
+          <t>Change in Revenue</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="11" t="inlineStr">
+        <is>
+          <t>Depreciation and Amortization</t>
+        </is>
+      </c>
+      <c r="C28" s="12" t="inlineStr">
+        <is>
+          <t>Depreciation and Amortization</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="11" t="inlineStr">
+        <is>
+          <t>CAPEX</t>
+        </is>
+      </c>
+      <c r="C29" s="12" t="inlineStr">
+        <is>
+          <t>CAPEX</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" s="11" t="inlineStr">
+        <is>
+          <t>Growth CAPEX</t>
+        </is>
+      </c>
+      <c r="C30" s="12" t="inlineStr">
+        <is>
+          <t>Growth CAPEX</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" s="13" t="inlineStr">
+        <is>
+          <t>Zero-growth CAPEX</t>
+        </is>
+      </c>
+      <c r="C31" s="14" t="inlineStr">
+        <is>
+          <t>Zero-growth CAPEX</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" s="15" t="inlineStr">
+        <is>
+          <t>Depreciation Adjustment</t>
+        </is>
+      </c>
+      <c r="C32" s="16" t="inlineStr">
+        <is>
+          <t>Depreciation Adjustment</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Retreiving tags from the financial statement
</commit_message>
<xml_diff>
--- a/edgar/EPV/DOMI.xlsx
+++ b/edgar/EPV/DOMI.xlsx
@@ -791,11 +791,7 @@
           <t>Premises and Equipment</t>
         </is>
       </c>
-      <c r="C24" s="10" t="inlineStr">
-        <is>
-          <t>Premises and Equipment</t>
-        </is>
-      </c>
+      <c r="C24" s="10" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="B25" s="11" t="inlineStr">
@@ -803,11 +799,7 @@
           <t>Current Year Revenue</t>
         </is>
       </c>
-      <c r="C25" s="12" t="inlineStr">
-        <is>
-          <t>Current Year Revenue</t>
-        </is>
-      </c>
+      <c r="C25" s="12" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="B26" s="11" t="inlineStr">
@@ -815,11 +807,7 @@
           <t>Prior Year Revenue</t>
         </is>
       </c>
-      <c r="C26" s="12" t="inlineStr">
-        <is>
-          <t>Prior Year Revenue</t>
-        </is>
-      </c>
+      <c r="C26" s="12" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="B27" s="11" t="inlineStr">
@@ -827,11 +815,7 @@
           <t>Change in Revenue</t>
         </is>
       </c>
-      <c r="C27" s="12" t="inlineStr">
-        <is>
-          <t>Change in Revenue</t>
-        </is>
-      </c>
+      <c r="C27" s="12" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="B28" s="11" t="inlineStr">
@@ -839,11 +823,7 @@
           <t>Depreciation and Amortization</t>
         </is>
       </c>
-      <c r="C28" s="12" t="inlineStr">
-        <is>
-          <t>Depreciation and Amortization</t>
-        </is>
-      </c>
+      <c r="C28" s="12" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="B29" s="11" t="inlineStr">
@@ -851,11 +831,7 @@
           <t>CAPEX</t>
         </is>
       </c>
-      <c r="C29" s="12" t="inlineStr">
-        <is>
-          <t>CAPEX</t>
-        </is>
-      </c>
+      <c r="C29" s="12" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="B30" s="11" t="inlineStr">
@@ -863,11 +839,7 @@
           <t>Growth CAPEX</t>
         </is>
       </c>
-      <c r="C30" s="12" t="inlineStr">
-        <is>
-          <t>Growth CAPEX</t>
-        </is>
-      </c>
+      <c r="C30" s="12" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="B31" s="13" t="inlineStr">
@@ -875,11 +847,7 @@
           <t>Zero-growth CAPEX</t>
         </is>
       </c>
-      <c r="C31" s="14" t="inlineStr">
-        <is>
-          <t>Zero-growth CAPEX</t>
-        </is>
-      </c>
+      <c r="C31" s="14" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="B32" s="15" t="inlineStr">
@@ -887,11 +855,7 @@
           <t>Depreciation Adjustment</t>
         </is>
       </c>
-      <c r="C32" s="16" t="inlineStr">
-        <is>
-          <t>Depreciation Adjustment</t>
-        </is>
-      </c>
+      <c r="C32" s="16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>